<commit_message>
Aggiunti Filtri su lista coupon
</commit_message>
<xml_diff>
--- a/Ore_su_custom backup.xlsx
+++ b/Ore_su_custom backup.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="138">
   <si>
     <t>Data</t>
   </si>
@@ -401,6 +401,39 @@
   </si>
   <si>
     <t>Salvataggio dei cli da elenco_coupon.php (work in progress)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salvataggio dei cli da elenco_coupon.php </t>
+  </si>
+  <si>
+    <t>Selezione multipa black-list da file</t>
+  </si>
+  <si>
+    <t>Acconto di 250€ (Tot 1250)</t>
+  </si>
+  <si>
+    <t>Acconto di 250€ (Tot 1500)</t>
+  </si>
+  <si>
+    <t>Acconto di 250€ (Tot 1750)</t>
+  </si>
+  <si>
+    <t>Modifica DB con aggiunta di only_export_Cli alla tabella users</t>
+  </si>
+  <si>
+    <t>Colloquio con vitaliano, analisi e interfacciamento con Daniele</t>
+  </si>
+  <si>
+    <t>Creazione utente e modifiche a coupon.php</t>
+  </si>
+  <si>
+    <t>Modifiche a Reatiler_panel.php; Creata user/statistichecoupon.php; Nuovi file per snellire codice UserPHPFunctions.php, RetailerPHPFunctions.php, AdminPHPFunctions.php</t>
+  </si>
+  <si>
+    <t>Publicazione e verifiche di funzionamento</t>
+  </si>
+  <si>
+    <t>Progettazione, concordazione con Vitaliano e Modifica (gestita in PHP) a selectTypeOfCli_mf e selectTypeOfCliMatch_mf che ora visualizza contenuti diversi per i clienti Standard+ListeCli</t>
   </si>
 </sst>
 </file>
@@ -12611,10 +12644,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12660,7 +12693,7 @@
       </c>
       <c r="G3" s="3">
         <f>SUMPRODUCT(B4:B1002,--(WEEKDAY(A4:A1002,2)&lt;6))</f>
-        <v>69</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -12690,7 +12723,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM(G3:G4)</f>
-        <v>69</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -12725,7 +12758,7 @@
       </c>
       <c r="G7">
         <f>G5*G6</f>
-        <v>1725</v>
+        <v>2450</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -12970,7 +13003,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>44089</v>
       </c>
@@ -12981,7 +13014,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>44090</v>
       </c>
@@ -12992,7 +13025,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>44091</v>
       </c>
@@ -13003,7 +13036,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>44092</v>
       </c>
@@ -13011,11 +13044,122 @@
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
+        <v>44096</v>
+      </c>
+      <c r="B37" s="2">
+        <v>3</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
+        <v>44097</v>
+      </c>
+      <c r="B38" s="2">
+        <v>4</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="11">
+        <v>44120</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="11">
+        <v>44153</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="11">
+        <v>44179</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="11">
+        <v>44180</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="11">
+        <v>44181</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="11">
+        <v>44182</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="11">
+        <v>44183</v>
+      </c>
+      <c r="B45">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="11">
+        <v>44186</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="11">
+        <v>44194</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>137</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>